<commit_message>
Fin des grilles aleatoire
</commit_message>
<xml_diff>
--- a/doc/journal de travail/journal de travail-Mikael.Juillet.xlsx
+++ b/doc/journal de travail/journal de travail-Mikael.Juillet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Clion_Exercises\Bataille navale\Bataille-Navale\doc\journal de travail\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A875FDB8-F4F1-4F9E-9AD6-26A0655D9DBA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3EC4519-218A-4379-866B-04792151AB54}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="53">
   <si>
     <t>Date</t>
   </si>
@@ -178,6 +178,12 @@
   </si>
   <si>
     <t>tentative de création de fonction rasemblant les différentes gilles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.25 h </t>
+  </si>
+  <si>
+    <t>fin de la construction des choix aléatoire de grille.</t>
   </si>
 </sst>
 </file>
@@ -343,20 +349,20 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -641,7 +647,7 @@
   <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -666,15 +672,15 @@
       <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14" t="s">
+      <c r="F1" s="15"/>
+      <c r="G1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
       <c r="J1" s="16"/>
       <c r="K1" s="9" t="s">
         <v>21</v>
@@ -693,22 +699,22 @@
       <c r="D2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
       <c r="K2" s="10">
         <v>3</v>
       </c>
-      <c r="L2" s="17" t="s">
+      <c r="L2" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:14" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
@@ -723,16 +729,16 @@
       <c r="D3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13" t="s">
+      <c r="F3" s="14"/>
+      <c r="G3" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
       <c r="K3" s="10">
         <v>3</v>
       </c>
@@ -750,14 +756,14 @@
       <c r="D4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
       <c r="K4" s="10">
         <v>3</v>
       </c>
@@ -775,14 +781,14 @@
       <c r="D5" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
       <c r="K5" s="11">
         <v>3</v>
       </c>
@@ -800,16 +806,16 @@
       <c r="D6" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13" t="s">
+      <c r="F6" s="14"/>
+      <c r="G6" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
       <c r="K6" s="11">
         <v>3</v>
       </c>
@@ -827,16 +833,16 @@
       <c r="D7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13" t="s">
+      <c r="F7" s="14"/>
+      <c r="G7" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
       <c r="K7" s="11">
         <v>3</v>
       </c>
@@ -854,14 +860,14 @@
       <c r="D8" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="E8" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
       <c r="K8" s="11">
         <v>4</v>
       </c>
@@ -879,14 +885,14 @@
       <c r="D9" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
       <c r="K9" s="11">
         <v>4</v>
       </c>
@@ -904,14 +910,14 @@
       <c r="D10" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E10" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
       <c r="K10" s="11">
         <v>4</v>
       </c>
@@ -929,16 +935,16 @@
       <c r="D11" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E11" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13" t="s">
+      <c r="F11" s="14"/>
+      <c r="G11" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
       <c r="K11" s="11">
         <v>4</v>
       </c>
@@ -956,16 +962,16 @@
       <c r="D12" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="13" t="s">
+      <c r="E12" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13" t="s">
+      <c r="F12" s="14"/>
+      <c r="G12" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
       <c r="K12" s="11">
         <v>4</v>
       </c>
@@ -983,14 +989,14 @@
       <c r="D13" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="E13" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
       <c r="K13" s="11">
         <v>5</v>
       </c>
@@ -1008,14 +1014,14 @@
       <c r="D14" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="13" t="s">
+      <c r="E14" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
       <c r="K14" s="11">
         <v>5</v>
       </c>
@@ -1033,16 +1039,16 @@
       <c r="D15" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E15" s="13" t="s">
+      <c r="E15" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13" t="s">
+      <c r="F15" s="14"/>
+      <c r="G15" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
       <c r="K15" s="11">
         <v>5</v>
       </c>
@@ -1060,14 +1066,14 @@
       <c r="D16" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E16" s="13" t="s">
+      <c r="E16" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
       <c r="K16" s="11">
         <v>5</v>
       </c>
@@ -1085,14 +1091,14 @@
       <c r="D17" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E17" s="13" t="s">
+      <c r="E17" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
       <c r="K17" s="11">
         <v>5</v>
       </c>
@@ -1110,16 +1116,16 @@
       <c r="D18" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E18" s="13" t="s">
+      <c r="E18" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13" t="s">
+      <c r="F18" s="14"/>
+      <c r="G18" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
       <c r="K18" s="11">
         <v>5</v>
       </c>
@@ -1137,16 +1143,16 @@
       <c r="D19" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E19" s="13" t="s">
+      <c r="E19" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13" t="s">
+      <c r="F19" s="14"/>
+      <c r="G19" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
       <c r="K19" s="11">
         <v>5</v>
       </c>
@@ -1164,14 +1170,14 @@
       <c r="D20" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E20" s="13" t="s">
+      <c r="E20" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
       <c r="K20" s="11">
         <v>6</v>
       </c>
@@ -1189,14 +1195,14 @@
       <c r="D21" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E21" s="13" t="s">
+      <c r="E21" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
       <c r="K21" s="11">
         <v>6</v>
       </c>
@@ -1214,14 +1220,14 @@
       <c r="D22" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E22" s="13" t="s">
+      <c r="E22" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
       <c r="K22" s="11">
         <v>6</v>
       </c>
@@ -1239,42 +1245,54 @@
       <c r="D23" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E23" s="13" t="s">
+      <c r="E23" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="14"/>
       <c r="K23" s="11">
         <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="13"/>
-      <c r="K24" s="11"/>
+      <c r="A24" s="8">
+        <v>43915</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="14"/>
+      <c r="K24" s="11">
+        <v>7</v>
+      </c>
     </row>
     <row r="25" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="5"/>
       <c r="D25" s="7"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="13"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14"/>
       <c r="K25" s="11"/>
     </row>
     <row r="26" spans="1:11" ht="15" x14ac:dyDescent="0.25">
@@ -1282,12 +1300,12 @@
       <c r="B26" s="4"/>
       <c r="C26" s="5"/>
       <c r="D26" s="7"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="13"/>
-      <c r="J26" s="13"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="14"/>
       <c r="K26" s="11"/>
     </row>
     <row r="27" spans="1:11" ht="15" x14ac:dyDescent="0.25">
@@ -1295,33 +1313,38 @@
       <c r="B27" s="4"/>
       <c r="C27" s="5"/>
       <c r="D27" s="7"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="13"/>
-      <c r="I27" s="13"/>
-      <c r="J27" s="13"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="14"/>
+      <c r="J27" s="14"/>
       <c r="K27" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="L2:N2"/>
-    <mergeCell ref="G10:J10"/>
-    <mergeCell ref="G11:J11"/>
-    <mergeCell ref="G12:J12"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="G27:J27"/>
-    <mergeCell ref="G16:J16"/>
-    <mergeCell ref="G17:J17"/>
-    <mergeCell ref="G18:J18"/>
-    <mergeCell ref="G19:J19"/>
-    <mergeCell ref="G20:J20"/>
-    <mergeCell ref="G21:J21"/>
-    <mergeCell ref="G22:J22"/>
-    <mergeCell ref="G23:J23"/>
-    <mergeCell ref="G24:J24"/>
-    <mergeCell ref="G25:J25"/>
-    <mergeCell ref="G26:J26"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:J15"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
     <mergeCell ref="E26:F26"/>
     <mergeCell ref="E27:F27"/>
     <mergeCell ref="G1:J1"/>
@@ -1338,28 +1361,23 @@
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="G9:J9"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:J15"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="G27:J27"/>
+    <mergeCell ref="G16:J16"/>
+    <mergeCell ref="G17:J17"/>
+    <mergeCell ref="G18:J18"/>
+    <mergeCell ref="G19:J19"/>
+    <mergeCell ref="G20:J20"/>
+    <mergeCell ref="G21:J21"/>
+    <mergeCell ref="G22:J22"/>
+    <mergeCell ref="G23:J23"/>
+    <mergeCell ref="G24:J24"/>
+    <mergeCell ref="G25:J25"/>
+    <mergeCell ref="G26:J26"/>
+    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="G10:J10"/>
+    <mergeCell ref="G11:J11"/>
+    <mergeCell ref="G12:J12"/>
+    <mergeCell ref="G13:J13"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D27" xr:uid="{00000000-0002-0000-0000-000000000000}">

</xml_diff>